<commit_message>
add test file with vexing characters in worksheet names
</commit_message>
<xml_diff>
--- a/inst/sheets/gabe.xlsx
+++ b/inst/sheets/gabe.xlsx
@@ -12,10 +12,13 @@
     <workbookView xWindow="1340" yWindow="460" windowWidth="27360" windowHeight="15740" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="HiGabe!!!!" sheetId="1" r:id="rId1"/>
+    <sheet name="Gabe's S''heet" sheetId="2" r:id="rId1"/>
+    <sheet name="HiGabe!!!!" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName name="A_one" localSheetId="0">'Gabe''s S''''heet'!$A$1</definedName>
     <definedName name="A_one">'HiGabe!!!!'!$A$1</definedName>
+    <definedName name="numbers" localSheetId="0">'Gabe''s S''''heet'!$A$2:$A$6</definedName>
     <definedName name="numbers">'HiGabe!!!!'!$A$2:$A$6</definedName>
   </definedNames>
   <calcPr calcId="150000" concurrentCalc="0"/>
@@ -31,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
     <t>numbers</t>
   </si>
@@ -350,7 +353,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -387,4 +392,47 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>